<commit_message>
adicionando estadisticas a los informes xls
</commit_message>
<xml_diff>
--- a/docs/tablas-analisis/Deteccion de forma.xlsx
+++ b/docs/tablas-analisis/Deteccion de forma.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FARIAS\WORK\CODE\freelance\onelia\QUINO - Tablas para el analisis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FARIAS\WORK\CODE\freelance\onelia\Quino\docs\tablas-analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -439,16 +439,16 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
     <col min="6" max="6" width="24.42578125" customWidth="1"/>
     <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>

</xml_diff>